<commit_message>
Insere planilha atualizada em Dez/2023- coluna ano
</commit_message>
<xml_diff>
--- a/upload/doacoes-comodatos-amigo-estado-mg.xlsx
+++ b/upload/doacoes-comodatos-amigo-estado-mg.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Silviana\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Silviana\Documents\.CGE\transparencia-mg\doacoes-comodatos\upload\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7115AA5-3851-4046-99F3-AC8F19BC64A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43B0469D-A965-4D66-96E7-9C06DA0FC409}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2301,7 +2301,7 @@
     <t>1400.01.0047088/2023-81</t>
   </si>
   <si>
-    <t>ANO_DOACAO</t>
+    <t>ANO</t>
   </si>
 </sst>
 </file>
@@ -9133,24 +9133,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="7df2fe0d-3e60-40fa-bf24-b5a426674ce4" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="af419fe6-3565-4d45-8405-d6ecc8112a1f">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <SharedWithUsers xmlns="7df2fe0d-3e60-40fa-bf24-b5a426674ce4">
-      <UserInfo>
-        <DisplayName>Daiane de Lana Cordeiro (SCC)</DisplayName>
-        <AccountId>166</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100705F7D4F09D2214BAEED5F294F982B42" ma:contentTypeVersion="13" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="a35e5acbee7105b9a177237d01c14401">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7df2fe0d-3e60-40fa-bf24-b5a426674ce4" xmlns:ns3="af419fe6-3565-4d45-8405-d6ecc8112a1f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a062360c7726b2e2c976e717d8f1bb04" ns2:_="" ns3:_="">
     <xsd:import namespace="7df2fe0d-3e60-40fa-bf24-b5a426674ce4"/>
@@ -9373,6 +9355,24 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="7df2fe0d-3e60-40fa-bf24-b5a426674ce4" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="af419fe6-3565-4d45-8405-d6ecc8112a1f">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <SharedWithUsers xmlns="7df2fe0d-3e60-40fa-bf24-b5a426674ce4">
+      <UserInfo>
+        <DisplayName>Daiane de Lana Cordeiro (SCC)</DisplayName>
+        <AccountId>166</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -9383,17 +9383,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F58222C8-1C8B-4E78-89E3-CD0B83F8E964}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="7df2fe0d-3e60-40fa-bf24-b5a426674ce4"/>
-    <ds:schemaRef ds:uri="af419fe6-3565-4d45-8405-d6ecc8112a1f"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70AE8147-C619-4FBD-9AD2-2516BE5792AA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9412,6 +9401,17 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F58222C8-1C8B-4E78-89E3-CD0B83F8E964}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="7df2fe0d-3e60-40fa-bf24-b5a426674ce4"/>
+    <ds:schemaRef ds:uri="af419fe6-3565-4d45-8405-d6ecc8112a1f"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2BC91FC8-6F4E-46FE-B825-6AFFCCFCC249}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Revert "Insere planilha atualizada em Dez/2023- coluna ano"
This reverts commit 8a3c67088670366dfa8f8753d1dcf1b57be0d6be.
</commit_message>
<xml_diff>
--- a/upload/doacoes-comodatos-amigo-estado-mg.xlsx
+++ b/upload/doacoes-comodatos-amigo-estado-mg.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Silviana\Documents\.CGE\transparencia-mg\doacoes-comodatos\upload\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Silviana\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43B0469D-A965-4D66-96E7-9C06DA0FC409}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7115AA5-3851-4046-99F3-AC8F19BC64A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2301,7 +2301,7 @@
     <t>1400.01.0047088/2023-81</t>
   </si>
   <si>
-    <t>ANO</t>
+    <t>ANO_DOACAO</t>
   </si>
 </sst>
 </file>
@@ -9133,6 +9133,24 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="7df2fe0d-3e60-40fa-bf24-b5a426674ce4" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="af419fe6-3565-4d45-8405-d6ecc8112a1f">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <SharedWithUsers xmlns="7df2fe0d-3e60-40fa-bf24-b5a426674ce4">
+      <UserInfo>
+        <DisplayName>Daiane de Lana Cordeiro (SCC)</DisplayName>
+        <AccountId>166</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100705F7D4F09D2214BAEED5F294F982B42" ma:contentTypeVersion="13" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="a35e5acbee7105b9a177237d01c14401">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7df2fe0d-3e60-40fa-bf24-b5a426674ce4" xmlns:ns3="af419fe6-3565-4d45-8405-d6ecc8112a1f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a062360c7726b2e2c976e717d8f1bb04" ns2:_="" ns3:_="">
     <xsd:import namespace="7df2fe0d-3e60-40fa-bf24-b5a426674ce4"/>
@@ -9355,24 +9373,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="7df2fe0d-3e60-40fa-bf24-b5a426674ce4" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="af419fe6-3565-4d45-8405-d6ecc8112a1f">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <SharedWithUsers xmlns="7df2fe0d-3e60-40fa-bf24-b5a426674ce4">
-      <UserInfo>
-        <DisplayName>Daiane de Lana Cordeiro (SCC)</DisplayName>
-        <AccountId>166</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -9383,6 +9383,17 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F58222C8-1C8B-4E78-89E3-CD0B83F8E964}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="7df2fe0d-3e60-40fa-bf24-b5a426674ce4"/>
+    <ds:schemaRef ds:uri="af419fe6-3565-4d45-8405-d6ecc8112a1f"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70AE8147-C619-4FBD-9AD2-2516BE5792AA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9401,17 +9412,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F58222C8-1C8B-4E78-89E3-CD0B83F8E964}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="7df2fe0d-3e60-40fa-bf24-b5a426674ce4"/>
-    <ds:schemaRef ds:uri="af419fe6-3565-4d45-8405-d6ecc8112a1f"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2BC91FC8-6F4E-46FE-B825-6AFFCCFCC249}">
   <ds:schemaRefs>

</xml_diff>